<commit_message>
al 1/3de door table 2
</commit_message>
<xml_diff>
--- a/table 4.xlsx
+++ b/table 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5275acbae45a446/Documenten/2021-2022/semester 2/bachelorproject/our-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{E2D32DD8-50D4-44F0-B1F6-07D46F611349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F73331A-5183-4DFC-9A49-597A19DEBE6D}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{E2D32DD8-50D4-44F0-B1F6-07D46F611349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8D3A44F-CCF8-4AE3-9586-F4B4AEAAEAB6}"/>
   <bookViews>
-    <workbookView xWindow="-10296" yWindow="3864" windowWidth="18720" windowHeight="8964" xr2:uid="{61D800A1-E571-409C-956A-7E3FD9C63226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{61D800A1-E571-409C-956A-7E3FD9C63226}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Test scores</t>
   </si>
@@ -209,6 +209,9 @@
       </rPr>
       <t>*</t>
     </r>
+  </si>
+  <si>
+    <t>*p&lt;0.1; **p&lt;0.05; ***p&lt;0.01</t>
   </si>
 </sst>
 </file>
@@ -336,9 +339,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,6 +367,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E8831F-CD65-47CE-AA89-7F306C500D69}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -694,24 +697,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -719,25 +722,25 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>0.13300000000000001</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
@@ -745,16 +748,16 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -762,16 +765,16 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>-9.7000000000000003E-2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>-3.5000000000000003E-2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>-1.6E-2</v>
       </c>
     </row>
@@ -779,49 +782,49 @@
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>0.112</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>0.09</v>
       </c>
     </row>
@@ -829,16 +832,16 @@
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -846,16 +849,16 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>0.115</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
@@ -863,49 +866,49 @@
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>0.155</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>0.11700000000000001</v>
       </c>
     </row>
@@ -913,16 +916,16 @@
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -930,16 +933,16 @@
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
@@ -947,49 +950,49 @@
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>0.16700000000000001</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>-6.5000000000000002E-2</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>-1.7000000000000001E-2</v>
       </c>
     </row>
@@ -997,16 +1000,16 @@
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1014,16 +1017,16 @@
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="12">
         <v>0.109</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="13">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
@@ -1031,25 +1034,30 @@
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>